<commit_message>
1e19 breaks the analysis gem 1e18 is okay
</commit_message>
<xml_diff>
--- a/projects/SEB_Morris_2013.xlsx
+++ b/projects/SEB_Morris_2013.xlsx
@@ -6660,8 +6660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6964,7 +6964,7 @@
         <v>772</v>
       </c>
       <c r="B28" s="28">
-        <v>1E+20</v>
+        <v>1E+18</v>
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="33"/>

</xml_diff>

<commit_message>
update for testing guideline 14
</commit_message>
<xml_diff>
--- a/projects/SEB_Morris_2013.xlsx
+++ b/projects/SEB_Morris_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="23256" windowHeight="13176" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -6674,8 +6674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6912,7 +6912,7 @@
         <v>752</v>
       </c>
       <c r="B22" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
         <v>780</v>
@@ -6924,7 +6924,7 @@
         <v>753</v>
       </c>
       <c r="B23" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23" s="29" t="s">
         <v>584</v>
@@ -7200,7 +7200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>

</xml_diff>